<commit_message>
Update Review Comments Document.xlsx
Ver 3 with internal review comments
</commit_message>
<xml_diff>
--- a/Review Comments/Review Comments Document.xlsx
+++ b/Review Comments/Review Comments Document.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1-ITI\15- Quality Assurance\1- Workshop\1- GIT\GitHub\learning-hub\Review Comments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\Review Comments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE970FE-C0EB-493D-A748-CD5137FC15DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE8C964-210E-4E3D-A3A7-DCB459D7FB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{517ADA08-9008-4EF8-8B33-926C871191B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{517ADA08-9008-4EF8-8B33-926C871191B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="115">
   <si>
     <t>Doc Version</t>
   </si>
@@ -374,6 +374,66 @@
   <si>
     <t>Confirmed</t>
   </si>
+  <si>
+    <t>Class diagram</t>
+  </si>
+  <si>
+    <t>V1.1</t>
+  </si>
+  <si>
+    <t>what are set category() and getcategory() functions?</t>
+  </si>
+  <si>
+    <t>catgory has id or no?</t>
+  </si>
+  <si>
+    <t>recording class not a photo class.</t>
+  </si>
+  <si>
+    <t>the content it self in the (article-video-recording) classes not in content class?</t>
+  </si>
+  <si>
+    <t>Mohamed mazrouaa</t>
+  </si>
+  <si>
+    <t>Category class</t>
+  </si>
+  <si>
+    <t>Recording class</t>
+  </si>
+  <si>
+    <t>Content class</t>
+  </si>
+  <si>
+    <t>Justified</t>
+  </si>
+  <si>
+    <t>Flowchart should have an start and end</t>
+  </si>
+  <si>
+    <t>Alaa osama</t>
+  </si>
+  <si>
+    <t>user should choose from article or upload not ( article/video/record)</t>
+  </si>
+  <si>
+    <t>Add content Flow chart</t>
+  </si>
+  <si>
+    <t>Categories Flow chart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review comments </t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>18/3 comments need to be added</t>
+  </si>
+  <si>
+    <t>Review comments  document</t>
+  </si>
 </sst>
 </file>
 
@@ -382,7 +442,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,8 +473,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F2328"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,8 +530,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -490,11 +581,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,6 +659,75 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,27 +1044,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165473DF-4415-4360-A898-B8D88BBC8B39}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="118.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="48.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>44</v>
       </c>
@@ -891,7 +1077,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -920,7 +1106,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>46</v>
       </c>
@@ -949,7 +1135,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>46</v>
       </c>
@@ -978,7 +1164,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>46</v>
       </c>
@@ -1007,7 +1193,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>46</v>
       </c>
@@ -1036,7 +1222,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -1065,7 +1251,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>46</v>
       </c>
@@ -1094,7 +1280,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>46</v>
       </c>
@@ -1123,7 +1309,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
@@ -1152,7 +1338,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
@@ -1181,7 +1367,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>46</v>
       </c>
@@ -1210,7 +1396,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1221,7 +1407,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>47</v>
       </c>
@@ -1250,7 +1436,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>47</v>
       </c>
@@ -1279,7 +1465,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>47</v>
       </c>
@@ -1308,7 +1494,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>47</v>
       </c>
@@ -1337,7 +1523,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>47</v>
       </c>
@@ -1366,7 +1552,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>47</v>
       </c>
@@ -1395,7 +1581,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1406,7 +1592,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
@@ -1435,7 +1621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>46</v>
       </c>
@@ -1464,7 +1650,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
@@ -1493,7 +1679,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>46</v>
       </c>
@@ -1522,7 +1708,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>46</v>
       </c>
@@ -1551,7 +1737,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1562,7 +1748,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>65</v>
       </c>
@@ -1591,7 +1777,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>47</v>
       </c>
@@ -1620,7 +1806,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>47</v>
       </c>
@@ -1649,311 +1835,576 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+    <row r="30" spans="1:9" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+    </row>
+    <row r="31" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="18">
+        <v>30</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="19">
+        <v>45005</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="18">
+        <v>31</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="19">
+        <v>45005</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="18">
+        <v>32</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="19">
+        <v>45005</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="18">
+        <v>33</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="19">
+        <v>45005</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="25" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="28">
+        <v>34</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="30">
+        <v>45019</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="28">
+        <v>35</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="30">
+        <v>45019</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="28">
+        <v>36</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" s="30">
+        <v>45019</v>
+      </c>
+      <c r="F38" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="34" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+    </row>
+    <row r="40" spans="1:9" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="35">
+        <v>37</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="37">
+        <v>45023</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="H40" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+    </row>
+    <row r="42" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B42" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="13">
-        <v>30</v>
-      </c>
-      <c r="D31" s="14" t="s">
+      <c r="C42" s="13">
+        <v>38</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E42" s="15">
         <v>45081</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="13" t="s">
+      <c r="F42" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13" t="s">
+      <c r="H42" s="13"/>
+      <c r="I42" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+    <row r="43" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B43" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="13">
-        <v>31</v>
-      </c>
-      <c r="D32" s="13" t="s">
+      <c r="C43" s="13">
+        <v>39</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E43" s="15">
         <v>45081</v>
       </c>
-      <c r="F32" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="13" t="s">
+      <c r="F43" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13" t="s">
+      <c r="H43" s="13"/>
+      <c r="I43" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+    <row r="44" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B44" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="13">
-        <v>32</v>
-      </c>
-      <c r="D33" s="13" t="s">
+      <c r="C44" s="13">
+        <v>40</v>
+      </c>
+      <c r="D44" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E44" s="15">
         <v>45081</v>
       </c>
-      <c r="F33" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="13" t="s">
+      <c r="F44" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13" t="s">
+      <c r="H44" s="13"/>
+      <c r="I44" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+    <row r="45" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B45" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="13">
-        <v>33</v>
-      </c>
-      <c r="D34" s="13" t="s">
+      <c r="C45" s="13">
+        <v>41</v>
+      </c>
+      <c r="D45" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E45" s="15">
         <v>45081</v>
       </c>
-      <c r="F34" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="13" t="s">
+      <c r="F45" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13" t="s">
+      <c r="H45" s="13"/>
+      <c r="I45" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+    <row r="46" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B46" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="13">
-        <v>34</v>
-      </c>
-      <c r="D35" s="14" t="s">
+      <c r="C46" s="13">
+        <v>42</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E46" s="15">
         <v>45081</v>
       </c>
-      <c r="F35" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="13" t="s">
+      <c r="F46" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13" t="s">
+      <c r="H46" s="13"/>
+      <c r="I46" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+    <row r="47" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B47" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="13">
-        <v>35</v>
-      </c>
-      <c r="D36" s="13" t="s">
+      <c r="C47" s="13">
+        <v>43</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E47" s="15">
         <v>45081</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="13" t="s">
+      <c r="F47" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13" t="s">
+      <c r="H47" s="13"/>
+      <c r="I47" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+    <row r="48" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B48" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="13">
-        <v>36</v>
-      </c>
-      <c r="D37" s="14" t="s">
+      <c r="C48" s="13">
+        <v>44</v>
+      </c>
+      <c r="D48" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E48" s="15">
         <v>45081</v>
       </c>
-      <c r="F37" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="13" t="s">
+      <c r="F48" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13" t="s">
+      <c r="H48" s="13"/>
+      <c r="I48" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+    <row r="49" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B49" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="13">
-        <v>37</v>
-      </c>
-      <c r="D38" s="13" t="s">
+      <c r="C49" s="13">
+        <v>45</v>
+      </c>
+      <c r="D49" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E49" s="15">
         <v>45081</v>
       </c>
-      <c r="F38" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="13" t="s">
+      <c r="F49" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13" t="s">
+      <c r="H49" s="13"/>
+      <c r="I49" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+    <row r="50" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B50" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="13">
-        <v>38</v>
-      </c>
-      <c r="D39" s="13" t="s">
+      <c r="C50" s="13">
+        <v>46</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E50" s="15">
         <v>45081</v>
       </c>
-      <c r="F39" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="13" t="s">
+      <c r="F50" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13" t="s">
+      <c r="H50" s="13"/>
+      <c r="I50" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+    <row r="51" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B51" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="13">
-        <v>39</v>
-      </c>
-      <c r="D40" s="13" t="s">
+      <c r="C51" s="13">
+        <v>47</v>
+      </c>
+      <c r="D51" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E51" s="15">
         <v>45081</v>
       </c>
-      <c r="F40" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="13" t="s">
+      <c r="F51" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13" t="s">
+      <c r="H51" s="13"/>
+      <c r="I51" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+    <row r="52" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B52" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="13">
-        <v>40</v>
-      </c>
-      <c r="D41" s="13" t="s">
+      <c r="C52" s="13">
+        <v>48</v>
+      </c>
+      <c r="D52" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E52" s="15">
         <v>45081</v>
       </c>
-      <c r="F41" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G41" s="13" t="s">
+      <c r="F52" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13" t="s">
+      <c r="H52" s="13"/>
+      <c r="I52" s="13" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1961,6 +2412,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Srs and review comments update
Srs modifying some features due to Amr comments
Adding amr comments in review comments document
</commit_message>
<xml_diff>
--- a/Review Comments/Review Comments Document.xlsx
+++ b/Review Comments/Review Comments Document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\Review Comments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE8C964-210E-4E3D-A3A7-DCB459D7FB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A44B06F-4FF7-4305-BCDB-3D607891FA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{517ADA08-9008-4EF8-8B33-926C871191B2}"/>
   </bookViews>
@@ -19,17 +19,28 @@
     <definedName name="_Toc128090186" localSheetId="0">Sheet1!$G$5</definedName>
     <definedName name="_Toc128090188" localSheetId="0">Sheet1!$G$6</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="136">
   <si>
     <t>Doc Version</t>
   </si>
@@ -433,6 +444,70 @@
   </si>
   <si>
     <t>Review comments  document</t>
+  </si>
+  <si>
+    <t>Review comments</t>
+  </si>
+  <si>
+    <t>V 2</t>
+  </si>
+  <si>
+    <t>No evidence for internal reviews</t>
+  </si>
+  <si>
+    <t>Review comments document</t>
+  </si>
+  <si>
+    <t>V 3</t>
+  </si>
+  <si>
+    <t>Review sheet is too general</t>
+  </si>
+  <si>
+    <t>Not clear</t>
+  </si>
+  <si>
+    <t>Mazrouaa</t>
+  </si>
+  <si>
+    <t>Need to be discussed</t>
+  </si>
+  <si>
+    <t>SRS-ADD-004 :   How to verify that
+SRS-ADD-007</t>
+  </si>
+  <si>
+    <t>Add feature</t>
+  </si>
+  <si>
+    <t>SRS-ADD-011 SRS-ADD-012  :    no added value</t>
+  </si>
+  <si>
+    <t>Notification feature</t>
+  </si>
+  <si>
+    <t>SRS-NOTIFI-004  :    Will he get notification if any article is added? How will he regiseter?</t>
+  </si>
+  <si>
+    <t>Done/Need to be discussed</t>
+  </si>
+  <si>
+    <t>Design document</t>
+  </si>
+  <si>
+    <t>Design document not found</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Sequence diagram</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>One sequence diagram</t>
   </si>
 </sst>
 </file>
@@ -611,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -658,76 +733,79 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1044,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165473DF-4415-4360-A898-B8D88BBC8B39}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1060,22 +1138,22 @@
     <col min="6" max="6" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5546875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1835,281 +1913,281 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-    </row>
-    <row r="31" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
+    <row r="30" spans="1:9" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+    </row>
+    <row r="31" spans="1:9" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="17">
         <v>30</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="18">
         <v>45005</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="H31" s="18" t="s">
+      <c r="H31" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="I31" s="17" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+    <row r="32" spans="1:9" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="17">
         <v>31</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="18">
         <v>45005</v>
       </c>
-      <c r="F32" s="18" t="s">
+      <c r="F32" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
+      <c r="I32" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="17">
         <v>32</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E33" s="18">
         <v>45005</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G33" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I33" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+      <c r="I33" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="17">
         <v>33</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="18">
         <v>45005</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="G34" s="18" t="s">
+      <c r="G34" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H34" s="18" t="s">
+      <c r="H34" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I34" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="25" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I34" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="20"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="19"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="28" t="s">
+    <row r="36" spans="1:9" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="28">
+      <c r="C36" s="27">
         <v>34</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="29">
         <v>45019</v>
       </c>
-      <c r="F36" s="28" t="s">
+      <c r="F36" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="G36" s="28" t="s">
+      <c r="G36" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="H36" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="28" t="s">
+      <c r="I36" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="28">
+      <c r="C37" s="27">
         <v>35</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="29">
         <v>45019</v>
       </c>
-      <c r="F37" s="28" t="s">
+      <c r="F37" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="G37" s="28" t="s">
+      <c r="G37" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H37" s="28" t="s">
+      <c r="H37" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="I37" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="28" t="s">
+      <c r="I37" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="28">
+      <c r="C38" s="27">
         <v>36</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="E38" s="30">
+      <c r="E38" s="29">
         <v>45019</v>
       </c>
-      <c r="F38" s="28" t="s">
+      <c r="F38" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="G38" s="28" t="s">
+      <c r="G38" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H38" s="28" t="s">
+      <c r="H38" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="34" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-    </row>
-    <row r="40" spans="1:9" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="35" t="s">
+      <c r="I38" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+    </row>
+    <row r="40" spans="1:9" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="35">
+      <c r="C40" s="33">
         <v>37</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="E40" s="37">
+      <c r="E40" s="35">
         <v>45023</v>
       </c>
-      <c r="F40" s="35" t="s">
+      <c r="F40" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="G40" s="35" t="s">
+      <c r="G40" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="H40" s="38" t="s">
+      <c r="H40" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="38" t="s">
+      <c r="I40" s="36" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
     </row>
     <row r="42" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
@@ -2406,6 +2484,214 @@
       <c r="H52" s="13"/>
       <c r="I52" s="13" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="25"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+    </row>
+    <row r="54" spans="1:9" s="40" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="6">
+        <v>49</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="39">
+        <v>45033</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="40" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" s="6">
+        <v>50</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" s="39">
+        <v>45033</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="40" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="6">
+        <v>51</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E56" s="39">
+        <v>45033</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="40" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" s="6">
+        <v>52</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57" s="39">
+        <v>45033</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="40" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="6">
+        <v>53</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E58" s="39">
+        <v>45033</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="40" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" s="6">
+        <v>54</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" s="39">
+        <v>45033</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="40" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="6">
+        <v>55</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="39">
+        <v>45033</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some reviews and changing flow charts location
</commit_message>
<xml_diff>
--- a/Review Comments/Review Comments Document.xlsx
+++ b/Review Comments/Review Comments Document.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\Review Comments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AA8487-2680-488F-B49A-BCC9D03CEEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BC46F8-AAAB-4543-BAAE-DAF3A080D2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{517ADA08-9008-4EF8-8B33-926C871191B2}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="153">
   <si>
     <t>Doc Version</t>
   </si>
@@ -470,9 +470,6 @@
     <t>Mazrouaa</t>
   </si>
   <si>
-    <t>Need to be discussed</t>
-  </si>
-  <si>
     <t>SRS-ADD-004 :   How to verify that
 SRS-ADD-007</t>
   </si>
@@ -489,9 +486,6 @@
     <t>SRS-NOTIFI-004  :    Will he get notification if any article is added? How will he regiseter?</t>
   </si>
   <si>
-    <t>Done/Need to be discussed</t>
-  </si>
-  <si>
     <t>Design document</t>
   </si>
   <si>
@@ -520,6 +514,54 @@
   </si>
   <si>
     <t>Done with another way</t>
+  </si>
+  <si>
+    <t>alaa</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>hasnaa</t>
+  </si>
+  <si>
+    <t>all team members</t>
+  </si>
+  <si>
+    <t>moataz</t>
+  </si>
+  <si>
+    <t>Username validation-password validation not in the login diagram
+construct db function not found</t>
+  </si>
+  <si>
+    <t>sequence daigrams</t>
+  </si>
+  <si>
+    <t>name of the function
+delete icon appear</t>
+  </si>
+  <si>
+    <t>nada</t>
+  </si>
+  <si>
+    <t>query arrow and its result are in opposite directions
+database connection not connection</t>
+  </si>
+  <si>
+    <t>V 1</t>
+  </si>
+  <si>
+    <t>remove un needed features replace it with components</t>
+  </si>
+  <si>
+    <t>get content diagram</t>
+  </si>
+  <si>
+    <t>get article diagram</t>
+  </si>
+  <si>
+    <t>No.comments</t>
   </si>
 </sst>
 </file>
@@ -1140,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165473DF-4415-4360-A898-B8D88BBC8B39}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2258,9 +2300,11 @@
       <c r="G43" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H43" s="13"/>
+      <c r="H43" s="13" t="s">
+        <v>138</v>
+      </c>
       <c r="I43" s="13" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2285,9 +2329,11 @@
       <c r="G44" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="H44" s="13"/>
+      <c r="H44" s="13" t="s">
+        <v>138</v>
+      </c>
       <c r="I44" s="13" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2370,7 +2416,9 @@
       <c r="G47" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="H47" s="13"/>
+      <c r="H47" s="13" t="s">
+        <v>132</v>
+      </c>
       <c r="I47" s="13" t="s">
         <v>64</v>
       </c>
@@ -2401,7 +2449,7 @@
         <v>122</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2582,7 +2630,9 @@
       <c r="G55" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H55" s="6"/>
+      <c r="H55" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="I55" s="6" t="s">
         <v>121</v>
       </c>
@@ -2598,7 +2648,7 @@
         <v>51</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E56" s="38">
         <v>45033</v>
@@ -2607,7 +2657,7 @@
         <v>8</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>122</v>
@@ -2627,7 +2677,7 @@
         <v>52</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E57" s="38">
         <v>45033</v>
@@ -2636,13 +2686,13 @@
         <v>8</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>122</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="39" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2656,7 +2706,7 @@
         <v>53</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E58" s="38">
         <v>45033</v>
@@ -2665,27 +2715,27 @@
         <v>8</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="39" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C59" s="6">
         <v>54</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E59" s="38">
         <v>45033</v>
@@ -2694,25 +2744,27 @@
         <v>8</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="H59" s="6"/>
+        <v>130</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="I59" s="6" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="39" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C60" s="6">
         <v>55</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E60" s="38">
         <v>45033</v>
@@ -2721,26 +2773,28 @@
         <v>8</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="H60" s="6"/>
+        <v>130</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="I60" s="6" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:9" s="40" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B62" s="40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C62" s="40">
         <v>56</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E62" s="41">
         <v>45049</v>
@@ -2749,7 +2803,159 @@
         <v>122</v>
       </c>
       <c r="G62" s="40" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="H62" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="I62" s="40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:9" s="39" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="6">
+        <v>57</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="38">
+        <v>45054</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="39" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="6">
+        <v>58</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E65" s="38">
+        <v>45052</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="39" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C66" s="6">
+        <v>59</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E66" s="38">
+        <v>45052</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="39" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="6">
+        <v>60</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E67" s="38">
+        <v>45055</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="39" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" s="6">
+        <v>61</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E68" s="38">
+        <v>45057</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Execution , modifying design document adding bug report adding testcases in rtm .modifying code
</commit_message>
<xml_diff>
--- a/Review Comments/Review Comments Document.xlsx
+++ b/Review Comments/Review Comments Document.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad\Documents\GitHub\learning-hub\Review Comments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\Review Comments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF80052B-4A34-49B6-9341-5F4A7CDD663A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54693DF7-A460-4449-81BE-A2B1E6501646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="193">
   <si>
     <t xml:space="preserve"> Review Comments </t>
   </si>
@@ -660,6 +660,21 @@
   <si>
     <t>the steps of all testcases are not follow the same sequence</t>
   </si>
+  <si>
+    <t>Test Strategy</t>
+  </si>
+  <si>
+    <t>bugs life cycle will not contain deferred</t>
+  </si>
+  <si>
+    <t>Eng.Mohamed Hassan</t>
+  </si>
+  <si>
+    <t>defect management</t>
+  </si>
+  <si>
+    <t>Done(not missing)</t>
+  </si>
 </sst>
 </file>
 
@@ -668,7 +683,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,8 +742,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -807,6 +829,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -871,7 +899,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1044,14 +1072,23 @@
     <xf numFmtId="14" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1330,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B83" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+    <sheetView tabSelected="1" topLeftCell="B77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1351,17 +1388,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.8">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="15.6">
       <c r="A2" s="13" t="s">
@@ -3651,99 +3688,143 @@
       <c r="G91" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="H91" s="57"/>
-      <c r="I91" s="57"/>
-    </row>
-    <row r="92" spans="1:9" s="61" customFormat="1" ht="18">
+      <c r="H91" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="I91" s="66" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" s="60" customFormat="1" ht="18">
       <c r="A92" s="57" t="s">
         <v>155</v>
       </c>
       <c r="B92" s="57" t="s">
         <v>165</v>
       </c>
-      <c r="C92" s="61">
+      <c r="C92" s="60">
         <v>82</v>
       </c>
-      <c r="D92" s="62" t="s">
+      <c r="D92" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="E92" s="63">
+      <c r="E92" s="62">
         <v>45064</v>
       </c>
-      <c r="F92" s="61" t="s">
+      <c r="F92" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="G92" s="61" t="s">
+      <c r="G92" s="60" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="93" spans="1:9" s="61" customFormat="1" ht="18">
+    <row r="93" spans="1:9" s="60" customFormat="1" ht="18">
       <c r="A93" s="57" t="s">
         <v>155</v>
       </c>
       <c r="B93" s="57" t="s">
         <v>165</v>
       </c>
-      <c r="C93" s="61">
+      <c r="C93" s="60">
         <v>83</v>
       </c>
-      <c r="D93" s="62" t="s">
+      <c r="D93" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="E93" s="63">
+      <c r="E93" s="62">
         <v>45064</v>
       </c>
-      <c r="F93" s="61" t="s">
+      <c r="F93" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="G93" s="61" t="s">
+      <c r="G93" s="60" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="94" spans="1:9" s="61" customFormat="1" ht="18">
+    <row r="94" spans="1:9" s="60" customFormat="1" ht="18">
       <c r="A94" s="57" t="s">
         <v>155</v>
       </c>
       <c r="B94" s="57" t="s">
         <v>165</v>
       </c>
-      <c r="C94" s="61">
+      <c r="C94" s="60">
         <v>84</v>
       </c>
-      <c r="D94" s="62" t="s">
+      <c r="D94" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="E94" s="63">
+      <c r="E94" s="62">
         <v>45064</v>
       </c>
-      <c r="F94" s="61" t="s">
+      <c r="F94" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="G94" s="61" t="s">
+      <c r="G94" s="60" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="95" spans="1:9" s="61" customFormat="1" ht="18">
+    <row r="95" spans="1:9" s="60" customFormat="1" ht="18">
       <c r="A95" s="57" t="s">
         <v>155</v>
       </c>
       <c r="B95" s="57" t="s">
         <v>165</v>
       </c>
-      <c r="C95" s="61">
+      <c r="C95" s="60">
         <v>85</v>
       </c>
-      <c r="D95" s="62" t="s">
+      <c r="D95" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="E95" s="63">
+      <c r="E95" s="62">
         <v>45064</v>
       </c>
-      <c r="F95" s="61" t="s">
+      <c r="F95" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="G95" s="61" t="s">
+      <c r="G95" s="60" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="2" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A96" s="48"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="49"/>
+      <c r="E96" s="50"/>
+      <c r="F96" s="48"/>
+      <c r="G96" s="48"/>
+      <c r="H96" s="48"/>
+      <c r="I96" s="48"/>
+    </row>
+    <row r="97" spans="1:9" s="64" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A97" s="64" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="C97" s="64">
+        <v>82</v>
+      </c>
+      <c r="D97" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="E97" s="65">
+        <v>45058</v>
+      </c>
+      <c r="F97" s="64" t="s">
+        <v>190</v>
+      </c>
+      <c r="G97" s="64" t="s">
+        <v>191</v>
+      </c>
+      <c r="H97" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="I97" s="64" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3751,6 +3832,6 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>